<commit_message>
Added Update and Certificate
</commit_message>
<xml_diff>
--- a/Project1 - CalculateClientSecurityHash/Data/Config.xlsx
+++ b/Project1 - CalculateClientSecurityHash/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RPA\UiPath\CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RPA\UiPath\RPA_DeveloperAdvanced\Project1 - CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE20354-AD41-4044-88D6-0B9A4A5EE2B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7B62F5-F7AC-4A5B-8B7E-3E2CCCCB76D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>number of retries</t>
   </si>
   <si>
-    <t>msedge</t>
-  </si>
-  <si>
     <t>process automation will be on web apps, thus only edge is required</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
   </si>
   <si>
     <t>RefColumn</t>
-  </si>
-  <si>
-    <t>ExceptionsMailAddress</t>
   </si>
   <si>
     <t>ExMailAddress</t>
@@ -252,6 +246,12 @@
   </si>
   <si>
     <t>CalculateClientSecurityHash, Unanticipated system exception found.</t>
+  </si>
+  <si>
+    <t>Acme_ExMailAddress</t>
+  </si>
+  <si>
+    <t>msedge,EXCEL</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -743,7 +743,7 @@
     </row>
     <row r="2" spans="1:26" ht="26.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>35</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -765,7 +765,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>21</v>
@@ -786,23 +786,23 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1804,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1916,10 +1916,10 @@
         <v>41</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -1928,37 +1928,37 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C17" s="7"/>
     </row>
@@ -1968,37 +1968,37 @@
     </row>
     <row r="19" spans="1:3" ht="60">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" ht="30">
       <c r="A20" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="60">
       <c r="A21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" ht="30">
       <c r="A22" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="7"/>
     </row>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" s="5">
         <v>3</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3052,7 +3052,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="19.5" customHeight="1"/>
@@ -3117,10 +3117,10 @@
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>31</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>31</v>

</xml_diff>